<commit_message>
Replace 'é' and 'è' with 'e'
</commit_message>
<xml_diff>
--- a/dataset_clean_1.xlsx
+++ b/dataset_clean_1.xlsx
@@ -26,6 +26,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -38,6 +39,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -50,6 +52,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -62,6 +65,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -74,6 +78,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -86,6 +91,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -98,6 +104,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -110,6 +117,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -122,6 +130,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -134,6 +143,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -146,6 +156,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -158,6 +169,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -170,6 +182,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -182,6 +195,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -194,6 +208,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -206,6 +221,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -218,6 +234,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -230,6 +247,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -242,6 +260,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -254,6 +273,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -266,6 +286,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -278,6 +299,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -290,6 +312,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -302,6 +325,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -314,6 +338,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -326,6 +351,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -338,6 +364,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -350,6 +377,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -362,6 +390,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -374,6 +403,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -386,6 +416,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -398,6 +429,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -410,6 +442,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -422,6 +455,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -434,6 +468,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -446,6 +481,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -458,6 +494,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -470,6 +507,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -482,6 +520,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -494,6 +533,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -506,6 +546,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -518,6 +559,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -530,6 +572,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -542,6 +585,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -554,6 +598,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -566,6 +611,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -578,6 +624,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -590,6 +637,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -602,6 +650,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -614,6 +663,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -626,6 +676,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -638,6 +689,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -650,6 +702,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -662,6 +715,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -674,6 +728,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -686,6 +741,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -698,6 +754,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -710,6 +767,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -722,6 +780,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -734,6 +793,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -746,6 +806,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -758,6 +819,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -770,6 +832,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -782,6 +845,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -794,6 +858,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -806,6 +871,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -818,6 +884,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -830,6 +897,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -842,6 +910,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -854,6 +923,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -866,6 +936,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -878,6 +949,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -890,6 +962,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -902,6 +975,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -914,6 +988,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -926,6 +1001,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -938,6 +1014,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -950,6 +1027,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -962,6 +1040,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -974,6 +1053,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -986,6 +1066,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -998,6 +1079,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1010,6 +1092,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1022,6 +1105,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1034,6 +1118,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1046,6 +1131,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1058,6 +1144,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1070,6 +1157,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1082,6 +1170,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1094,6 +1183,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1106,6 +1196,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1118,6 +1209,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1130,6 +1222,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1142,6 +1235,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1154,6 +1248,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1166,6 +1261,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1178,6 +1274,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1190,6 +1287,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1202,6 +1300,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1214,6 +1313,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1226,6 +1326,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1238,6 +1339,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1250,6 +1352,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1262,6 +1365,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1274,6 +1378,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1286,6 +1391,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1298,6 +1404,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1310,6 +1417,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1322,6 +1430,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1334,6 +1443,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1346,6 +1456,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1358,6 +1469,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1370,6 +1482,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1382,6 +1495,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1394,6 +1508,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1406,6 +1521,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1418,6 +1534,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1430,6 +1547,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1442,6 +1560,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1454,6 +1573,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1466,6 +1586,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1478,6 +1599,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1490,6 +1612,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1502,6 +1625,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1514,6 +1638,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1526,6 +1651,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1538,6 +1664,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Le participant a mis à jour cette valeur.</t>
         </r>
@@ -1559,12 +1686,6 @@
     <t>Quel est votre sexe?</t>
   </si>
   <si>
-    <t>Quel est votre niveau d'étude?</t>
-  </si>
-  <si>
-    <t>Quelle est votre école / faculté</t>
-  </si>
-  <si>
     <t>Est-ce que vous suivez/avez suivi des 2 ?</t>
   </si>
   <si>
@@ -1574,39 +1695,12 @@
     <t>Quels appareils utilisez-vous ?</t>
   </si>
   <si>
-    <t>Quelle est votre plateforme préférée ?</t>
-  </si>
-  <si>
-    <t>Quels sont les problèmes techniques auxquels vous faites face ? [Perte de connexion ou débit faible]</t>
-  </si>
-  <si>
-    <t>Combien de séance vous étudiez par semaine ?</t>
-  </si>
-  <si>
     <t>Durant l'enseignement à distance: [Les devoirs sont devenus nombreux]</t>
   </si>
   <si>
-    <t>Qu'est ce que vous préférez? [Sous les conditions actuelles]</t>
-  </si>
-  <si>
     <t>Les cours sont plus sous forme de: [Cours interactive]</t>
   </si>
   <si>
-    <t>Comment cette situation 2t affecter votre classement pour le choix de filière, mobilité ou double diplomation</t>
-  </si>
-  <si>
-    <t>Quels sont les problèmes techniques auxquels vous faites face ? [Manipulation des plateformes]</t>
-  </si>
-  <si>
-    <t>Quels sont les problèmes techniques auxquels vous faites face ? [Coupure d'électricité]</t>
-  </si>
-  <si>
-    <t>Quels sont les problèmes techniques auxquels vous faites face ? [blocage de l'ordinateur]</t>
-  </si>
-  <si>
-    <t>Quels sont les problèmes techniques auxquels vous faites face ? [Indisponibilité des appareils]</t>
-  </si>
-  <si>
     <t>Durant l'enseignement à distance: [Les cours sont plus difficile à suvire]</t>
   </si>
   <si>
@@ -1616,120 +1710,30 @@
     <t>Durant l'enseignement à distance: [Vous assimilez les cours]</t>
   </si>
   <si>
-    <t>Les cours sont plus sous forme de: [Visioconférence]</t>
-  </si>
-  <si>
-    <t>Les cours sont plus sous forme de: [Cours PDF/PPT téléchargeable]</t>
-  </si>
-  <si>
-    <t>Les cours sont plus sous forme de: [Vidéo téléchargeable]</t>
-  </si>
-  <si>
-    <t>Qu'est ce que vous-préférez le plus: [Cours interactive]</t>
-  </si>
-  <si>
-    <t>Qu'est ce que vous-préférez le plus: [Visioconférence]</t>
-  </si>
-  <si>
-    <t>Qu'est ce que vous-préférez le plus: [Cours PDF/PPT téléchargeable]</t>
-  </si>
-  <si>
-    <t>Qu'est ce que vous-préférez le plus: [Vidéo téléchargeable]</t>
-  </si>
-  <si>
     <t xml:space="preserve"> [Les devoirs sont devenus nombreux]</t>
   </si>
   <si>
-    <t>Qu'est ce que vous pensez des affirmations suivantes?  [Les enseignants sont bien formés pour assurer des 2]</t>
-  </si>
-  <si>
     <t>Qu'est ce que vous pensez des affirmations suivantes?  [Les enseignants respectent les horaires]</t>
   </si>
   <si>
-    <t>Qu'est ce que vous pensez des affirmations suivantes?  [Les élèves respectent les horaires]</t>
-  </si>
-  <si>
-    <t>Qu'est ce que vous pensez des affirmations suivantes?  [Les enseignants s'assurent de l'assiduité des élèves]</t>
-  </si>
-  <si>
-    <t>Qu'est ce que vous pensez des affirmations suivantes?  [Vous avez une excellente assiduité durant les 2]</t>
-  </si>
-  <si>
-    <t>Qu'est ce que vous pensez des affirmations suivantes?  [Vous gérer bien votre temps]</t>
-  </si>
-  <si>
     <t>Qu'est ce que vous pensez des affirmations suivantes?  [Vous dormez plus]</t>
   </si>
   <si>
-    <t>Les enseignants s'assurent de l'assiduité des élèves à l'aide : [Des quiz]</t>
-  </si>
-  <si>
-    <t>Les enseignants s'assurent de l'assiduité des élèves à l'aide : [D'appel]</t>
-  </si>
-  <si>
-    <t>Les enseignants s'assurent de l'assiduité des élèves à l'aide : [Des questions durant le cours]</t>
-  </si>
-  <si>
-    <t>Qu'est ce que vous pensez des affirmations suivantes?  [Les enseignants sont bien formés pour assurer des 2?]</t>
-  </si>
-  <si>
-    <t>Comment vous impacte cette situation actuelle? [Productivité]</t>
-  </si>
-  <si>
     <t>Comment vous impacte cette situation actuelle? [Innovation]</t>
   </si>
   <si>
-    <t>Comment vous impacte cette situation actuelle? [Créativité]</t>
-  </si>
-  <si>
     <t>Comment vous impacte cette situation actuelle? [Stress]</t>
   </si>
   <si>
-    <t>Comment vous impacte cette situation actuelle? [Anxiété]</t>
-  </si>
-  <si>
     <t>Comment vous impacte cette situation actuelle? [Ennui]</t>
   </si>
   <si>
-    <t>Comment vous impacte cette situation actuelle? [Dépression]</t>
-  </si>
-  <si>
     <t>Comment vous impacte cette situation actuelle? [Concentration]</t>
   </si>
   <si>
-    <t>Préférez-vous les examens: [En présentiel]</t>
-  </si>
-  <si>
-    <t>Préférez-vous les examens: [Questions ouvertes]</t>
-  </si>
-  <si>
-    <t>Préférez-vous les examens: [Questions à choix multiple]</t>
-  </si>
-  <si>
-    <t>Préférez-vous les examens: [Vidéo téléchargeable]</t>
-  </si>
-  <si>
-    <t>Préférez-vous les examens: [Projet]</t>
-  </si>
-  <si>
-    <t>Préférez-vous les examens: [Excercices]</t>
-  </si>
-  <si>
-    <t>Préférez-vous les examens: [Evaluation orale (à distance)]</t>
-  </si>
-  <si>
-    <t>Préférez-vous les examens: [À distance]</t>
-  </si>
-  <si>
-    <t>Qu'est ce que vous préférez? [Après amélioration des conditions de l'enseignement à distance]</t>
-  </si>
-  <si>
     <t>Adresse e-mail</t>
   </si>
   <si>
-    <t>Les enseignants s'assurent de l'assiduité des élèves è l'aide : [Vidéo téléchargeable]</t>
-  </si>
-  <si>
     <t>2, 3</t>
   </si>
   <si>
@@ -2016,6 +2020,129 @@
   </si>
   <si>
     <t>1, 2, 3</t>
+  </si>
+  <si>
+    <t>Quel est votre niveau d'etude?</t>
+  </si>
+  <si>
+    <t>Quelle est votre ecole / faculte</t>
+  </si>
+  <si>
+    <t>Quelle est votre plateforme preferee ?</t>
+  </si>
+  <si>
+    <t>Combien de seance vous etudiez par semaine ?</t>
+  </si>
+  <si>
+    <t>Qu'est ce que vous preferez? [Sous les conditions actuelles]</t>
+  </si>
+  <si>
+    <t>Les cours sont plus sous forme de: [Visioconference]</t>
+  </si>
+  <si>
+    <t>Les cours sont plus sous forme de: [Cours PDF/PPT telechargeable]</t>
+  </si>
+  <si>
+    <t>Les cours sont plus sous forme de: [Video telechargeable]</t>
+  </si>
+  <si>
+    <t>Qu'est ce que vous-preferez le plus: [Cours interactive]</t>
+  </si>
+  <si>
+    <t>Qu'est ce que vous-preferez le plus: [Visioconference]</t>
+  </si>
+  <si>
+    <t>Qu'est ce que vous-preferez le plus: [Cours PDF/PPT telechargeable]</t>
+  </si>
+  <si>
+    <t>Qu'est ce que vous-preferez le plus: [Video telechargeable]</t>
+  </si>
+  <si>
+    <t>Qu'est ce que vous pensez des affirmations suivantes?  [Les enseignants sont bien formes pour assurer des 2]</t>
+  </si>
+  <si>
+    <t>Qu'est ce que vous pensez des affirmations suivantes?  [Vous avez une excellente assiduite durant les 2]</t>
+  </si>
+  <si>
+    <t>Qu'est ce que vous pensez des affirmations suivantes?  [Vous gerer bien votre temps]</t>
+  </si>
+  <si>
+    <t>Qu'est ce que vous pensez des affirmations suivantes?  [Les enseignants sont bien formes pour assurer des 2?]</t>
+  </si>
+  <si>
+    <t>Comment vous impacte cette situation actuelle? [Productivite]</t>
+  </si>
+  <si>
+    <t>Comment vous impacte cette situation actuelle? [Creativite]</t>
+  </si>
+  <si>
+    <t>Comment vous impacte cette situation actuelle? [Anxiete]</t>
+  </si>
+  <si>
+    <t>Comment vous impacte cette situation actuelle? [Depression]</t>
+  </si>
+  <si>
+    <t>Preferez-vous les examens: [En presentiel]</t>
+  </si>
+  <si>
+    <t>Preferez-vous les examens: [Questions ouvertes]</t>
+  </si>
+  <si>
+    <t>Preferez-vous les examens: [Questions à choix multiple]</t>
+  </si>
+  <si>
+    <t>Preferez-vous les examens: [Video telechargeable]</t>
+  </si>
+  <si>
+    <t>Preferez-vous les examens: [Projet]</t>
+  </si>
+  <si>
+    <t>Preferez-vous les examens: [Excercices]</t>
+  </si>
+  <si>
+    <t>Preferez-vous les examens: [Evaluation orale (à distance)]</t>
+  </si>
+  <si>
+    <t>Preferez-vous les examens: [À distance]</t>
+  </si>
+  <si>
+    <t>Quels sont les problemes techniques auxquels vous faites face ? [Perte de connexion ou debit faible]</t>
+  </si>
+  <si>
+    <t>Comment cette situation 2t affecter votre classement pour le choix de filiere, mobilite ou double diplomation</t>
+  </si>
+  <si>
+    <t>Quels sont les problemes techniques auxquels vous faites face ? [Manipulation des plateformes]</t>
+  </si>
+  <si>
+    <t>Quels sont les problemes techniques auxquels vous faites face ? [Coupure d'electricite]</t>
+  </si>
+  <si>
+    <t>Quels sont les problemes techniques auxquels vous faites face ? [blocage de l'ordinateur]</t>
+  </si>
+  <si>
+    <t>Quels sont les problemes techniques auxquels vous faites face ? [Indisponibilite des appareils]</t>
+  </si>
+  <si>
+    <t>Qu'est ce que vous pensez des affirmations suivantes?  [Les eleves respectent les horaires]</t>
+  </si>
+  <si>
+    <t>Qu'est ce que vous pensez des affirmations suivantes?  [Les enseignants s'assurent de l'assiduite des eleves]</t>
+  </si>
+  <si>
+    <t>Les enseignants s'assurent de l'assiduite des eleves à l'aide : [Des quiz]</t>
+  </si>
+  <si>
+    <t>Les enseignants s'assurent de l'assiduite des eleves à l'aide : [D'appel]</t>
+  </si>
+  <si>
+    <t>Les enseignants s'assurent de l'assiduite des eleves à l'aide : [Des questions durant le cours]</t>
+  </si>
+  <si>
+    <t>Qu'est ce que vous preferez? [Apres amelioration des conditions de l'enseignement à distance]</t>
+  </si>
+  <si>
+    <t>Les enseignants s'assurent de l'assiduite des eleves e l'aide : [Video telechargeable]</t>
   </si>
 </sst>
 </file>
@@ -2025,7 +2152,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2039,6 +2166,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2335,178 +2468,178 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>115</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>116</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="M1" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="O1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="V1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="W1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="AE1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AF1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="AK1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="AL1" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="AS1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="AU1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="AV1" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="AW1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="AX1" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="AY1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="AZ1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="BA1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="BB1" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="BC1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="BD1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="BE1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="BF1" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="BG1" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="BH1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AR1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AS1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AT1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AU1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AV1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AW1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AX1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AY1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AZ1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="BA1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="BB1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="BC1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="BD1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="BE1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="BF1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="BG1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="BH1" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="BI1" s="3" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:61" x14ac:dyDescent="0.2">
@@ -2529,10 +2662,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I2" s="2">
         <v>1</v>
@@ -2676,7 +2809,7 @@
         <v>1</v>
       </c>
       <c r="BH2" s="3" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:61" x14ac:dyDescent="0.2">
@@ -2699,10 +2832,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I3" s="3">
         <v>3</v>
@@ -2850,7 +2983,7 @@
         <v>2</v>
       </c>
       <c r="BH3" s="3" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="BI3" s="5"/>
     </row>
@@ -2874,10 +3007,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I4" s="2">
         <v>1</v>
@@ -3021,7 +3154,7 @@
         <v>1</v>
       </c>
       <c r="BH4" s="3" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:61" x14ac:dyDescent="0.2">
@@ -3044,10 +3177,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I5" s="2">
         <v>1</v>
@@ -3191,7 +3324,7 @@
         <v>2</v>
       </c>
       <c r="BH5" s="3" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:61" x14ac:dyDescent="0.2">
@@ -3217,7 +3350,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I6" s="2">
         <v>1</v>
@@ -3361,7 +3494,7 @@
         <v>1</v>
       </c>
       <c r="BH6" s="3" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:61" x14ac:dyDescent="0.2">
@@ -3531,7 +3664,7 @@
         <v>2</v>
       </c>
       <c r="BH7" s="3" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:61" x14ac:dyDescent="0.2">
@@ -3557,7 +3690,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I8" s="2">
         <v>1</v>
@@ -3701,7 +3834,7 @@
         <v>1</v>
       </c>
       <c r="BH8" s="3" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:61" x14ac:dyDescent="0.2">
@@ -3871,7 +4004,7 @@
         <v>1</v>
       </c>
       <c r="BH9" s="3" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:61" x14ac:dyDescent="0.2">
@@ -4041,7 +4174,7 @@
         <v>1</v>
       </c>
       <c r="BH10" s="3" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:61" x14ac:dyDescent="0.2">
@@ -4064,7 +4197,7 @@
         <v>2</v>
       </c>
       <c r="BH11" s="3" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:61" x14ac:dyDescent="0.2">
@@ -4090,7 +4223,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I12" s="2">
         <v>1</v>
@@ -4234,7 +4367,7 @@
         <v>2</v>
       </c>
       <c r="BH12" s="3" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:61" x14ac:dyDescent="0.2">
@@ -4257,13 +4390,13 @@
         <v>1</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="J13" s="2">
         <v>3</v>
@@ -4404,7 +4537,7 @@
         <v>1</v>
       </c>
       <c r="BH13" s="3" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:61" x14ac:dyDescent="0.2">
@@ -4427,10 +4560,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>151</v>
+        <v>110</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I14" s="2">
         <v>3</v>
@@ -4574,7 +4707,7 @@
         <v>1</v>
       </c>
       <c r="BH14" s="3" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:61" x14ac:dyDescent="0.2">
@@ -4744,7 +4877,7 @@
         <v>2</v>
       </c>
       <c r="BH15" s="3" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:61" x14ac:dyDescent="0.2">
@@ -4767,10 +4900,10 @@
         <v>1</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I16" s="2">
         <v>1</v>
@@ -4914,7 +5047,7 @@
         <v>1</v>
       </c>
       <c r="BH16" s="3" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:61" x14ac:dyDescent="0.2">
@@ -4937,10 +5070,10 @@
         <v>1</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I17" s="2">
         <v>1</v>
@@ -5084,7 +5217,7 @@
         <v>2</v>
       </c>
       <c r="BH17" s="2" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:61" x14ac:dyDescent="0.2">
@@ -5107,10 +5240,10 @@
         <v>1</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I18" s="2">
         <v>1</v>
@@ -5254,7 +5387,7 @@
         <v>1</v>
       </c>
       <c r="BH18" s="3" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:61" x14ac:dyDescent="0.2">
@@ -5277,7 +5410,7 @@
         <v>2</v>
       </c>
       <c r="BH19" s="3" t="s">
-        <v>80</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:61" x14ac:dyDescent="0.2">
@@ -5300,7 +5433,7 @@
         <v>2</v>
       </c>
       <c r="BH20" s="3" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:61" x14ac:dyDescent="0.2">
@@ -5323,10 +5456,10 @@
         <v>1</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I21" s="2">
         <v>3</v>
@@ -5470,7 +5603,7 @@
         <v>2</v>
       </c>
       <c r="BH21" s="3" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:61" x14ac:dyDescent="0.2">
@@ -5496,7 +5629,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I22" s="2">
         <v>1</v>
@@ -5640,7 +5773,7 @@
         <v>1</v>
       </c>
       <c r="BH22" s="2" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:61" x14ac:dyDescent="0.2">
@@ -5663,7 +5796,7 @@
         <v>2</v>
       </c>
       <c r="BH23" s="3" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:61" x14ac:dyDescent="0.2">
@@ -5686,7 +5819,7 @@
         <v>2</v>
       </c>
       <c r="BH24" s="3" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:61" x14ac:dyDescent="0.2">
@@ -5709,7 +5842,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="H25" s="3">
         <v>2</v>
@@ -5860,7 +5993,7 @@
         <v>2</v>
       </c>
       <c r="BH25" s="3" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="BI25" s="5"/>
     </row>
@@ -5884,7 +6017,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="H26" s="2">
         <v>2</v>
@@ -6031,7 +6164,7 @@
         <v>1</v>
       </c>
       <c r="BH26" s="3" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:61" x14ac:dyDescent="0.2">
@@ -6054,7 +6187,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="H27" s="2">
         <v>2</v>
@@ -6201,7 +6334,7 @@
         <v>1</v>
       </c>
       <c r="BH27" s="2" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:61" x14ac:dyDescent="0.2">
@@ -6224,10 +6357,10 @@
         <v>1</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I28" s="2">
         <v>3</v>
@@ -6371,7 +6504,7 @@
         <v>2</v>
       </c>
       <c r="BH28" s="3" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:61" x14ac:dyDescent="0.2">
@@ -6394,10 +6527,10 @@
         <v>1</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I29" s="2">
         <v>1</v>
@@ -6541,7 +6674,7 @@
         <v>1</v>
       </c>
       <c r="BH29" s="3" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:61" x14ac:dyDescent="0.2">
@@ -6564,13 +6697,13 @@
         <v>1</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="J30" s="2">
         <v>5</v>
@@ -6711,7 +6844,7 @@
         <v>2</v>
       </c>
       <c r="BH30" s="3" t="s">
-        <v>91</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:61" x14ac:dyDescent="0.2">
@@ -6734,7 +6867,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="H31" s="2">
         <v>2</v>
@@ -6881,7 +7014,7 @@
         <v>1</v>
       </c>
       <c r="BH31" s="3" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:61" x14ac:dyDescent="0.2">
@@ -6904,10 +7037,10 @@
         <v>1</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I32" s="2">
         <v>3</v>
@@ -7051,7 +7184,7 @@
         <v>1</v>
       </c>
       <c r="BH32" s="3" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:60" x14ac:dyDescent="0.2">
@@ -7074,10 +7207,10 @@
         <v>1</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I33" s="2">
         <v>1</v>
@@ -7221,7 +7354,7 @@
         <v>1</v>
       </c>
       <c r="BH33" s="3" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:60" x14ac:dyDescent="0.2">
@@ -7244,10 +7377,10 @@
         <v>1</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>152</v>
+        <v>111</v>
       </c>
       <c r="I34" s="2">
         <v>1</v>
@@ -7391,7 +7524,7 @@
         <v>1</v>
       </c>
       <c r="BH34" s="2" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:60" x14ac:dyDescent="0.2">
@@ -7414,7 +7547,7 @@
         <v>1</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="H35" s="2">
         <v>2</v>
@@ -7561,7 +7694,7 @@
         <v>2</v>
       </c>
       <c r="BH35" s="3" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:60" x14ac:dyDescent="0.2">
@@ -7584,10 +7717,10 @@
         <v>1</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I36" s="2">
         <v>3</v>
@@ -7731,7 +7864,7 @@
         <v>1</v>
       </c>
       <c r="BH36" s="3" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:60" x14ac:dyDescent="0.2">
@@ -7754,10 +7887,10 @@
         <v>1</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I37" s="2">
         <v>1</v>
@@ -7901,7 +8034,7 @@
         <v>1</v>
       </c>
       <c r="BH37" s="3" t="s">
-        <v>98</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:60" x14ac:dyDescent="0.2">
@@ -7924,7 +8057,7 @@
         <v>2</v>
       </c>
       <c r="BH38" s="3" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:60" x14ac:dyDescent="0.2">
@@ -7947,7 +8080,7 @@
         <v>1</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="H39" s="2">
         <v>2</v>
@@ -8094,7 +8227,7 @@
         <v>1</v>
       </c>
       <c r="BH39" s="3" t="s">
-        <v>100</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:60" x14ac:dyDescent="0.2">
@@ -8117,154 +8250,154 @@
         <v>1</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="H40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I40" s="2">
+        <v>1</v>
+      </c>
+      <c r="J40" s="2">
+        <v>2</v>
+      </c>
+      <c r="K40" s="2">
+        <v>1</v>
+      </c>
+      <c r="L40" s="2">
+        <v>4</v>
+      </c>
+      <c r="M40" s="2">
+        <v>2</v>
+      </c>
+      <c r="N40" s="2">
+        <v>4</v>
+      </c>
+      <c r="O40" s="3">
+        <v>1</v>
+      </c>
+      <c r="P40" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q40" s="2">
+        <v>5</v>
+      </c>
+      <c r="R40" s="2">
+        <v>3</v>
+      </c>
+      <c r="S40" s="2">
+        <v>4</v>
+      </c>
+      <c r="T40" s="2">
+        <v>1</v>
+      </c>
+      <c r="U40" s="2">
+        <v>4</v>
+      </c>
+      <c r="V40" s="2">
+        <v>4</v>
+      </c>
+      <c r="W40" s="2">
+        <v>2</v>
+      </c>
+      <c r="X40" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y40" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z40" s="2">
+        <v>5</v>
+      </c>
+      <c r="AA40" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB40" s="2">
+        <v>4</v>
+      </c>
+      <c r="AC40" s="2">
+        <v>4</v>
+      </c>
+      <c r="AE40" s="2">
+        <v>4</v>
+      </c>
+      <c r="AF40" s="2">
+        <v>4</v>
+      </c>
+      <c r="AG40" s="2">
+        <v>4</v>
+      </c>
+      <c r="AH40" s="2">
+        <v>4</v>
+      </c>
+      <c r="AI40" s="2">
+        <v>4</v>
+      </c>
+      <c r="AJ40" s="2">
+        <v>4</v>
+      </c>
+      <c r="AK40" s="2">
+        <v>5</v>
+      </c>
+      <c r="AL40" s="2">
+        <v>2</v>
+      </c>
+      <c r="AM40" s="2">
+        <v>5</v>
+      </c>
+      <c r="AN40" s="2">
+        <v>3</v>
+      </c>
+      <c r="AP40" s="2">
+        <v>3</v>
+      </c>
+      <c r="AQ40" s="2">
+        <v>1</v>
+      </c>
+      <c r="AR40" s="2">
+        <v>3</v>
+      </c>
+      <c r="AS40" s="2">
+        <v>4</v>
+      </c>
+      <c r="AT40" s="2">
+        <v>3</v>
+      </c>
+      <c r="AU40" s="2">
+        <v>5</v>
+      </c>
+      <c r="AV40" s="2">
+        <v>3</v>
+      </c>
+      <c r="AW40" s="2">
+        <v>1</v>
+      </c>
+      <c r="AY40" s="2">
+        <v>4</v>
+      </c>
+      <c r="AZ40" s="2">
+        <v>2</v>
+      </c>
+      <c r="BB40" s="2">
+        <v>2</v>
+      </c>
+      <c r="BC40" s="2">
+        <v>4</v>
+      </c>
+      <c r="BD40" s="2">
+        <v>5</v>
+      </c>
+      <c r="BE40" s="2">
+        <v>1</v>
+      </c>
+      <c r="BF40" s="2">
+        <v>5</v>
+      </c>
+      <c r="BG40" s="2">
+        <v>1</v>
+      </c>
+      <c r="BH40" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="I40" s="2">
-        <v>1</v>
-      </c>
-      <c r="J40" s="2">
-        <v>2</v>
-      </c>
-      <c r="K40" s="2">
-        <v>1</v>
-      </c>
-      <c r="L40" s="2">
-        <v>4</v>
-      </c>
-      <c r="M40" s="2">
-        <v>2</v>
-      </c>
-      <c r="N40" s="2">
-        <v>4</v>
-      </c>
-      <c r="O40" s="3">
-        <v>1</v>
-      </c>
-      <c r="P40" s="2">
-        <v>4</v>
-      </c>
-      <c r="Q40" s="2">
-        <v>5</v>
-      </c>
-      <c r="R40" s="2">
-        <v>3</v>
-      </c>
-      <c r="S40" s="2">
-        <v>4</v>
-      </c>
-      <c r="T40" s="2">
-        <v>1</v>
-      </c>
-      <c r="U40" s="2">
-        <v>4</v>
-      </c>
-      <c r="V40" s="2">
-        <v>4</v>
-      </c>
-      <c r="W40" s="2">
-        <v>2</v>
-      </c>
-      <c r="X40" s="2">
-        <v>2</v>
-      </c>
-      <c r="Y40" s="2">
-        <v>2</v>
-      </c>
-      <c r="Z40" s="2">
-        <v>5</v>
-      </c>
-      <c r="AA40" s="2">
-        <v>2</v>
-      </c>
-      <c r="AB40" s="2">
-        <v>4</v>
-      </c>
-      <c r="AC40" s="2">
-        <v>4</v>
-      </c>
-      <c r="AE40" s="2">
-        <v>4</v>
-      </c>
-      <c r="AF40" s="2">
-        <v>4</v>
-      </c>
-      <c r="AG40" s="2">
-        <v>4</v>
-      </c>
-      <c r="AH40" s="2">
-        <v>4</v>
-      </c>
-      <c r="AI40" s="2">
-        <v>4</v>
-      </c>
-      <c r="AJ40" s="2">
-        <v>4</v>
-      </c>
-      <c r="AK40" s="2">
-        <v>5</v>
-      </c>
-      <c r="AL40" s="2">
-        <v>2</v>
-      </c>
-      <c r="AM40" s="2">
-        <v>5</v>
-      </c>
-      <c r="AN40" s="2">
-        <v>3</v>
-      </c>
-      <c r="AP40" s="2">
-        <v>3</v>
-      </c>
-      <c r="AQ40" s="2">
-        <v>1</v>
-      </c>
-      <c r="AR40" s="2">
-        <v>3</v>
-      </c>
-      <c r="AS40" s="2">
-        <v>4</v>
-      </c>
-      <c r="AT40" s="2">
-        <v>3</v>
-      </c>
-      <c r="AU40" s="2">
-        <v>5</v>
-      </c>
-      <c r="AV40" s="2">
-        <v>3</v>
-      </c>
-      <c r="AW40" s="2">
-        <v>1</v>
-      </c>
-      <c r="AY40" s="2">
-        <v>4</v>
-      </c>
-      <c r="AZ40" s="2">
-        <v>2</v>
-      </c>
-      <c r="BB40" s="2">
-        <v>2</v>
-      </c>
-      <c r="BC40" s="2">
-        <v>4</v>
-      </c>
-      <c r="BD40" s="2">
-        <v>5</v>
-      </c>
-      <c r="BE40" s="2">
-        <v>1</v>
-      </c>
-      <c r="BF40" s="2">
-        <v>5</v>
-      </c>
-      <c r="BG40" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH40" s="3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:60" x14ac:dyDescent="0.2">
@@ -8287,10 +8420,10 @@
         <v>1</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I41" s="2">
         <v>1</v>
@@ -8434,7 +8567,7 @@
         <v>2</v>
       </c>
       <c r="BH41" s="3" t="s">
-        <v>102</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:60" x14ac:dyDescent="0.2">
@@ -8457,10 +8590,10 @@
         <v>1</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I42" s="2">
         <v>3</v>
@@ -8604,7 +8737,7 @@
         <v>1</v>
       </c>
       <c r="BH42" s="3" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:60" x14ac:dyDescent="0.2">
@@ -8630,7 +8763,7 @@
         <v>3</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I43" s="2">
         <v>3</v>
@@ -8774,7 +8907,7 @@
         <v>1</v>
       </c>
       <c r="BH43" s="3" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:60" x14ac:dyDescent="0.2">
@@ -8797,7 +8930,7 @@
         <v>1</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="H44" s="2">
         <v>2</v>
@@ -8944,7 +9077,7 @@
         <v>2</v>
       </c>
       <c r="BH44" s="3" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:60" x14ac:dyDescent="0.2">
@@ -8970,7 +9103,7 @@
         <v>1</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>152</v>
+        <v>111</v>
       </c>
       <c r="I45" s="2">
         <v>1</v>
@@ -9114,7 +9247,7 @@
         <v>1</v>
       </c>
       <c r="BH45" s="3" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:60" x14ac:dyDescent="0.2">
@@ -9137,7 +9270,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="H46" s="2">
         <v>3</v>
@@ -9284,7 +9417,7 @@
         <v>2</v>
       </c>
       <c r="BH46" s="2" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:60" x14ac:dyDescent="0.2">
@@ -9307,13 +9440,13 @@
         <v>1</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="H47" s="2">
         <v>2</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="J47" s="2">
         <v>2</v>
@@ -9454,7 +9587,7 @@
         <v>1</v>
       </c>
       <c r="BH47" s="3" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:60" x14ac:dyDescent="0.2">
@@ -9477,10 +9610,10 @@
         <v>1</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="I48" s="2">
         <v>3</v>
@@ -9624,7 +9757,7 @@
         <v>1</v>
       </c>
       <c r="BH48" s="3" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:60" x14ac:dyDescent="0.2">
@@ -9794,7 +9927,7 @@
         <v>2</v>
       </c>
       <c r="BH49" s="3" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:60" x14ac:dyDescent="0.2">
@@ -9817,7 +9950,7 @@
         <v>2</v>
       </c>
       <c r="BH50" s="3" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:60" x14ac:dyDescent="0.2">
@@ -9840,7 +9973,7 @@
         <v>1</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="H51" s="2">
         <v>2</v>
@@ -9987,7 +10120,7 @@
         <v>1</v>
       </c>
       <c r="BH51" s="3" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:60" x14ac:dyDescent="0.2">
@@ -10157,7 +10290,7 @@
         <v>1</v>
       </c>
       <c r="BH52" s="3" t="s">
-        <v>114</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:60" x14ac:dyDescent="0.2">
@@ -10180,10 +10313,10 @@
         <v>1</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I53" s="2">
         <v>3</v>
@@ -10327,7 +10460,7 @@
         <v>2</v>
       </c>
       <c r="BH53" s="3" t="s">
-        <v>115</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" spans="1:60" x14ac:dyDescent="0.2">
@@ -10350,13 +10483,13 @@
         <v>1</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="H54" s="2">
         <v>2</v>
       </c>
       <c r="I54" s="7" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="J54" s="2">
         <v>2</v>
@@ -10497,7 +10630,7 @@
         <v>2</v>
       </c>
       <c r="BH54" s="2" t="s">
-        <v>116</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:60" x14ac:dyDescent="0.2">
@@ -10667,7 +10800,7 @@
         <v>1</v>
       </c>
       <c r="BH55" s="3" t="s">
-        <v>117</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:60" x14ac:dyDescent="0.2">
@@ -10690,10 +10823,10 @@
         <v>1</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I56" s="2">
         <v>1</v>
@@ -10837,7 +10970,7 @@
         <v>2</v>
       </c>
       <c r="BH56" s="3" t="s">
-        <v>118</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:60" x14ac:dyDescent="0.2">
@@ -10860,10 +10993,10 @@
         <v>1</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>152</v>
+        <v>111</v>
       </c>
       <c r="I57" s="2">
         <v>1</v>
@@ -11007,7 +11140,7 @@
         <v>2</v>
       </c>
       <c r="BH57" s="3" t="s">
-        <v>119</v>
+        <v>78</v>
       </c>
     </row>
     <row r="58" spans="1:60" x14ac:dyDescent="0.2">
@@ -11030,7 +11163,7 @@
         <v>2</v>
       </c>
       <c r="BH58" s="3" t="s">
-        <v>120</v>
+        <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:60" x14ac:dyDescent="0.2">
@@ -11053,13 +11186,13 @@
         <v>1</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>153</v>
+        <v>112</v>
       </c>
       <c r="H59" s="2">
         <v>2</v>
       </c>
       <c r="I59" s="7" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="J59" s="2">
         <v>2</v>
@@ -11200,7 +11333,7 @@
         <v>2</v>
       </c>
       <c r="BH59" s="3" t="s">
-        <v>121</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60" spans="1:60" x14ac:dyDescent="0.2">
@@ -11223,10 +11356,10 @@
         <v>1</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I60" s="2">
         <v>3</v>
@@ -11370,7 +11503,7 @@
         <v>1</v>
       </c>
       <c r="BH60" s="3" t="s">
-        <v>122</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:60" x14ac:dyDescent="0.2">
@@ -11396,7 +11529,7 @@
         <v>1</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I61" s="2">
         <v>3</v>
@@ -11540,7 +11673,7 @@
         <v>1</v>
       </c>
       <c r="BH61" s="3" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
     </row>
     <row r="62" spans="1:60" x14ac:dyDescent="0.2">
@@ -11563,7 +11696,7 @@
         <v>1</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="H62" s="2">
         <v>2</v>
@@ -11710,7 +11843,7 @@
         <v>2</v>
       </c>
       <c r="BH62" s="3" t="s">
-        <v>124</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:60" x14ac:dyDescent="0.2">
@@ -11733,7 +11866,7 @@
         <v>2</v>
       </c>
       <c r="BH63" s="3" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
     </row>
     <row r="64" spans="1:60" x14ac:dyDescent="0.2">
@@ -11903,7 +12036,7 @@
         <v>1</v>
       </c>
       <c r="BH64" s="3" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:60" x14ac:dyDescent="0.2">
@@ -11929,7 +12062,7 @@
         <v>1</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I65" s="2">
         <v>1</v>
@@ -12073,7 +12206,7 @@
         <v>1</v>
       </c>
       <c r="BH65" s="3" t="s">
-        <v>127</v>
+        <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:60" x14ac:dyDescent="0.2">
@@ -12096,7 +12229,7 @@
         <v>2</v>
       </c>
       <c r="BH66" s="3" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
     </row>
     <row r="67" spans="1:60" x14ac:dyDescent="0.2">
@@ -12119,7 +12252,7 @@
         <v>2</v>
       </c>
       <c r="BH67" s="3" t="s">
-        <v>129</v>
+        <v>88</v>
       </c>
     </row>
     <row r="68" spans="1:60" x14ac:dyDescent="0.2">
@@ -12289,7 +12422,7 @@
         <v>1</v>
       </c>
       <c r="BH68" s="3" t="s">
-        <v>130</v>
+        <v>89</v>
       </c>
     </row>
     <row r="69" spans="1:60" x14ac:dyDescent="0.2">
@@ -12312,7 +12445,7 @@
         <v>2</v>
       </c>
       <c r="BH69" s="3" t="s">
-        <v>131</v>
+        <v>90</v>
       </c>
     </row>
     <row r="70" spans="1:60" x14ac:dyDescent="0.2">
@@ -12335,10 +12468,10 @@
         <v>1</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I70" s="2">
         <v>3</v>
@@ -12482,7 +12615,7 @@
         <v>1</v>
       </c>
       <c r="BH70" s="3" t="s">
-        <v>132</v>
+        <v>91</v>
       </c>
     </row>
     <row r="71" spans="1:60" x14ac:dyDescent="0.2">
@@ -12508,7 +12641,7 @@
         <v>1</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I71" s="2">
         <v>1</v>
@@ -12652,7 +12785,7 @@
         <v>2</v>
       </c>
       <c r="BH71" s="3" t="s">
-        <v>133</v>
+        <v>92</v>
       </c>
     </row>
     <row r="72" spans="1:60" x14ac:dyDescent="0.2">
@@ -12675,7 +12808,7 @@
         <v>2</v>
       </c>
       <c r="BH72" s="3" t="s">
-        <v>134</v>
+        <v>93</v>
       </c>
     </row>
     <row r="73" spans="1:60" x14ac:dyDescent="0.2">
@@ -12698,7 +12831,7 @@
         <v>2</v>
       </c>
       <c r="BH73" s="2" t="s">
-        <v>135</v>
+        <v>94</v>
       </c>
     </row>
     <row r="74" spans="1:60" x14ac:dyDescent="0.2">
@@ -12721,10 +12854,10 @@
         <v>1</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I74" s="2">
         <v>1</v>
@@ -12868,7 +13001,7 @@
         <v>1</v>
       </c>
       <c r="BH74" s="3" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
     </row>
     <row r="75" spans="1:60" x14ac:dyDescent="0.2">
@@ -12891,7 +13024,7 @@
         <v>1</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="H75" s="2">
         <v>2</v>
@@ -13038,7 +13171,7 @@
         <v>1</v>
       </c>
       <c r="BH75" s="2" t="s">
-        <v>137</v>
+        <v>96</v>
       </c>
     </row>
     <row r="76" spans="1:60" x14ac:dyDescent="0.2">
@@ -13061,7 +13194,7 @@
         <v>1</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="H76" s="2">
         <v>2</v>
@@ -13208,7 +13341,7 @@
         <v>1</v>
       </c>
       <c r="BH76" s="3" t="s">
-        <v>138</v>
+        <v>97</v>
       </c>
     </row>
     <row r="77" spans="1:60" x14ac:dyDescent="0.2">
@@ -13378,7 +13511,7 @@
         <v>1</v>
       </c>
       <c r="BH77" s="2" t="s">
-        <v>139</v>
+        <v>98</v>
       </c>
     </row>
     <row r="78" spans="1:60" x14ac:dyDescent="0.2">
@@ -13407,7 +13540,7 @@
         <v>3</v>
       </c>
       <c r="I78" s="7" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="J78" s="2">
         <v>2</v>
@@ -13548,7 +13681,7 @@
         <v>1</v>
       </c>
       <c r="BH78" s="3" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
     </row>
     <row r="79" spans="1:60" x14ac:dyDescent="0.2">
@@ -13718,7 +13851,7 @@
         <v>2</v>
       </c>
       <c r="BH79" s="3" t="s">
-        <v>141</v>
+        <v>100</v>
       </c>
     </row>
     <row r="80" spans="1:60" x14ac:dyDescent="0.2">
@@ -13741,7 +13874,7 @@
         <v>2</v>
       </c>
       <c r="BH80" s="3" t="s">
-        <v>142</v>
+        <v>101</v>
       </c>
     </row>
     <row r="81" spans="1:60" x14ac:dyDescent="0.2">
@@ -13764,7 +13897,7 @@
         <v>1</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="H81" s="2">
         <v>2</v>
@@ -13911,7 +14044,7 @@
         <v>1</v>
       </c>
       <c r="BH81" s="3" t="s">
-        <v>143</v>
+        <v>102</v>
       </c>
     </row>
     <row r="82" spans="1:60" x14ac:dyDescent="0.2">
@@ -14081,7 +14214,7 @@
         <v>2</v>
       </c>
       <c r="BH82" s="3" t="s">
-        <v>144</v>
+        <v>103</v>
       </c>
     </row>
     <row r="83" spans="1:60" x14ac:dyDescent="0.2">
@@ -14104,7 +14237,7 @@
         <v>1</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="H83" s="2">
         <v>3</v>
@@ -14251,7 +14384,7 @@
         <v>1</v>
       </c>
       <c r="BH83" s="3" t="s">
-        <v>145</v>
+        <v>104</v>
       </c>
     </row>
     <row r="84" spans="1:60" x14ac:dyDescent="0.2">
@@ -14274,13 +14407,13 @@
         <v>1</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>154</v>
+        <v>113</v>
       </c>
       <c r="H84" s="2">
         <v>2</v>
       </c>
       <c r="I84" s="7" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="J84" s="2">
         <v>1</v>
@@ -14421,7 +14554,7 @@
         <v>2</v>
       </c>
       <c r="BH84" s="3" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="85" spans="1:60" x14ac:dyDescent="0.2">
@@ -14447,7 +14580,7 @@
         <v>5</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I85" s="2">
         <v>5</v>
@@ -14591,7 +14724,7 @@
         <v>2</v>
       </c>
       <c r="BH85" s="3" t="s">
-        <v>147</v>
+        <v>106</v>
       </c>
     </row>
     <row r="86" spans="1:60" x14ac:dyDescent="0.2">
@@ -14617,7 +14750,7 @@
         <v>1</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I86" s="2">
         <v>1</v>
@@ -14761,7 +14894,7 @@
         <v>2</v>
       </c>
       <c r="BH86" s="3" t="s">
-        <v>148</v>
+        <v>107</v>
       </c>
     </row>
     <row r="87" spans="1:60" x14ac:dyDescent="0.2">
@@ -14784,7 +14917,7 @@
         <v>2</v>
       </c>
       <c r="BH87" s="3" t="s">
-        <v>149</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>